<commit_message>
Entrega FInal Falta Conclusao
</commit_message>
<xml_diff>
--- a/Projeto 2/Annabelle_2.xlsx
+++ b/Projeto 2/Annabelle_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vf_ga\OneDrive\Documentos\2º Semestre Eng\Ciencia dos Dados\GIT\CienciaDosDados\Projeto 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="17D2D069EB89A04BA76C792A2316E95B668637CB" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{D4C2F4D2-8105-4E4A-AA63-82DF6B5C2D04}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="17D2D069EB89A04BA76C792A2316E95B668637CB" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{ED400F1D-6A95-4FEA-AD2B-98D70062C01F}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4178,7 +4178,7 @@
   <dimension ref="A1:B201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>